<commit_message>
Supervision section reformated in all versions
</commit_message>
<xml_diff>
--- a/data/supervision_eng_S.xlsx
+++ b/data/supervision_eng_S.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F9BBFF-6443-4FE9-B33A-DF8BE1886AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164F9947-C053-4180-A69B-3C7424AFD527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supervision" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>what</t>
   </si>
@@ -37,24 +37,12 @@
     <t>why</t>
   </si>
   <si>
-    <t>2013 - 2014</t>
-  </si>
-  <si>
     <t>2015 - 2018</t>
   </si>
   <si>
     <t>Professional Doctorate in Counselling Psychology</t>
   </si>
   <si>
-    <t>\href{https://www.uel.ac.uk/}{University of East London}, UK</t>
-  </si>
-  <si>
-    <t>\href{https://www.stir.ac.uk/}{University of Stirling}, UK</t>
-  </si>
-  <si>
-    <t>Supervised together with \href{https://www.scraigroberts.com/}{S Craig Roberts}</t>
-  </si>
-  <si>
     <t>Supervised together with Lisa Chiara Fellin</t>
   </si>
   <si>
@@ -67,16 +55,19 @@
     <t>\href{https://www.uv.es/}{Universitat de València}, Spain</t>
   </si>
   <si>
-    <t>Julia Sanz-Vidania</t>
-  </si>
-  <si>
-    <t>Psychological Research Methods (Evolutionary Psychology) MSc - \textbf{\textit{Distinction}}</t>
-  </si>
-  <si>
     <t>\href{https://www.researchgate.net/profile/Milena-Vasquez-Amezquita}{Milena Vásquez-Amézquita}</t>
   </si>
   <si>
-    <t>PhD in Neuroscience  - \textbf{\textit{Summa Cum Laude}}</t>
+    <t>PhD in Neuroscience</t>
+  </si>
+  <si>
+    <t>Thesis \textbf{(\textit{Summa Cum Laude})}: \textit{\href{http://hdl.handle.net/10550/67639}{Preferencias sexuales típicas y atípicas según sexo y edad de los estímulos: Utilidad de la técnica de rastreo ocular} [Typical and atypical sexual preferences according to sex and age of the stimuli: Usefulness of the eye tracking technique]}</t>
+  </si>
+  <si>
+    <t>\href{https://www.uel.ac.uk/}{U. of East London}, UK</t>
+  </si>
+  <si>
+    <t>Tésis: \textit{What sense do people make of the functions of their ’behaviours that may be causing problems in their everyday life’? A hybrid deductive/inductive template analysis}</t>
   </si>
 </sst>
 </file>
@@ -566,11 +557,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -929,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,54 +950,55 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>